<commit_message>
Turned backgroud image into place instead of pack turns out image have to be after Canv function added textbox for years added button to exit
</commit_message>
<xml_diff>
--- a/OUTPUT.xlsx
+++ b/OUTPUT.xlsx
@@ -14,69 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="26">
-  <si>
-    <t>Week1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">May  1 </t>
   </si>
   <si>
     <t>3 pm</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>G</t>
+    <t>Team One</t>
+  </si>
+  <si>
+    <t>Team Three</t>
+  </si>
+  <si>
+    <t>Team Five</t>
+  </si>
+  <si>
+    <t>Team Seven</t>
   </si>
   <si>
     <t>7 pm</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Week2</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>Week3</t>
-  </si>
-  <si>
-    <t>Week4</t>
-  </si>
-  <si>
-    <t>Week5</t>
-  </si>
-  <si>
-    <t>Week6</t>
-  </si>
-  <si>
-    <t>Week7</t>
+    <t>Team Nin</t>
+  </si>
+  <si>
+    <t>Team Two</t>
+  </si>
+  <si>
+    <t>Team Four</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May  2 </t>
+  </si>
+  <si>
+    <t>Team Six</t>
+  </si>
+  <si>
+    <t>Team Eight</t>
+  </si>
+  <si>
+    <t>Team Ten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May  8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May  9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 22 </t>
   </si>
   <si>
     <t>vs</t>
   </si>
   <si>
-    <t>K</t>
+    <t>Team Eleven</t>
   </si>
   <si>
     <t>at</t>
@@ -449,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -618,7 +618,7 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1652,19 +1652,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
         <v>19</v>
       </c>
       <c r="D78" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E78" t="s">
         <v>21</v>
       </c>
       <c r="F78" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1672,19 +1672,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
         <v>19</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
         <v>21</v>
       </c>
       <c r="F79" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1692,19 +1692,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" t="s">
-        <v>21</v>
-      </c>
-      <c r="F80" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1712,7 +1700,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" t="s">
+        <v>21</v>
+      </c>
+      <c r="F81" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1720,19 +1720,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
         <v>19</v>
       </c>
       <c r="D82" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E82" t="s">
         <v>21</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1740,38 +1740,18 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
         <v>19</v>
       </c>
       <c r="D83" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E83" t="s">
         <v>21</v>
       </c>
       <c r="F83" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="1">
-        <v>82</v>
-      </c>
-      <c r="B84" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" t="s">
-        <v>19</v>
-      </c>
-      <c r="D84" t="s">
-        <v>20</v>
-      </c>
-      <c r="E84" t="s">
-        <v>21</v>
-      </c>
-      <c r="F84" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>